<commit_message>
chinh sua logic kho va lo hang them chuc nang quan li nha cung cap #131
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_IJ\Project-LTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC030BD-7E76-469A-9BAB-90241A2C9548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E7A784-DE49-4357-9F7A-ED940F7304D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{127CE7C5-AD73-4B95-869C-9E17D6E38290}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{127CE7C5-AD73-4B95-869C-9E17D6E38290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +465,7 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="D2">
         <v>13000</v>
@@ -479,7 +479,7 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="D3">
         <v>13000</v>

</xml_diff>